<commit_message>
3 Pt Linearity Test
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -432,7 +432,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -762,7 +762,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -804,7 +804,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1.31802104279309e-06</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>6.34864375892577</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>-1.69889727685646e-06</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>-7.82851865175457</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.000222388359832818</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1057.59008402095</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1.67156856187751e-06</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>7.95532909968744</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1424,7 +1424,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.000231374756624682</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2038.39309588292</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>-1.01202052956844e-06</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>-8.93039299948133</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2.76084247607497e-07</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2.44818258734443</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1.16899232556872e-07</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>1.27059178656855</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1.83252930795797e-07</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>1.94799331459379</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>3.36818891729114e-07</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>3.59253724469407</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3056,12 +3056,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-3.48379580108469e-05</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-370.8319472873</t>
         </is>
       </c>
     </row>
@@ -3098,7 +3098,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3284,7 +3284,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3.98039650706417e-05</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>429.424281085316</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">

</xml_diff>